<commit_message>
IDEFICS-3 TOT_PA_AC:Algori. changes We will keep the sendentary for a while because other studies consider that in their calculation but we need to discuss that further on tuesday
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_IDEFICS_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_IDEFICS_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6415B0CF-4691-4649-B83F-69A2A1FE5872}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F758C5A3-1F95-41A7-8F85-7D38A68BEF4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,13 +505,13 @@
       TRUE ~ NA_integer_)</t>
   </si>
   <si>
-    <t>((1.5 * SED)/60 + (1.5 * LPA)/60 + (3 * MPA)/60 + (6 * VPA)/60) / 7</t>
-  </si>
-  <si>
     <t>phys_activ;leis_activ</t>
   </si>
   <si>
     <t>(4 * phys_activ + 1.5 * leis_activ) / 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((1.5 * SED)/60 + (1.5 * LPA)/60 + (3 * MPA)/60 + (6 * VPA)/60) </t>
   </si>
 </sst>
 </file>
@@ -952,7 +952,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,13 +1119,13 @@
         <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>143</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>135</v>
@@ -1229,7 +1229,7 @@
         <v>143</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>135</v>

</xml_diff>